<commit_message>
Take Date values directly
</commit_message>
<xml_diff>
--- a/test/out/style.xlsx
+++ b/test/out/style.xlsx
@@ -438,7 +438,9 @@
       <c r="J3"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4"/>
+      <c r="A4">
+        <v>42755.20833333333</v>
+      </c>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>

</xml_diff>